<commit_message>
Minor changes to Iteration 1
</commit_message>
<xml_diff>
--- a/Iteration1/defect_log-Iteration1.xlsx
+++ b/Iteration1/defect_log-Iteration1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\OneDrive - Ara Institute of Canterbury\Year 2\Semester 1\Software Engineering\Assignment 1\Iteration1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="11_9772094146B369BB7D2AB030540DAC71AB463A6C" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{E7C17077-06D0-4C24-80E9-F2D8D6C43FE0}"/>
+  <xr:revisionPtr revIDLastSave="58" documentId="11_9772094146B369BB7D2AB030540DAC71AB463A6C" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{055E8DB6-8EFA-4CE8-A009-5D195005EDF2}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="435" windowWidth="19875" windowHeight="7710" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="73">
   <si>
     <t>PSP Defect Recording Log</t>
   </si>
@@ -604,15 +604,9 @@
     <t>Amit / Luofeng</t>
   </si>
   <si>
-    <t>WT/MC/WE</t>
-  </si>
-  <si>
     <t>Was comparing a string with a number. ParseInt() used to fix. E.g. "this.guess === randomNum"</t>
   </si>
   <si>
-    <t>MI</t>
-  </si>
-  <si>
     <t>User could input non-numeric characters. Input type changed to "number"</t>
   </si>
   <si>
@@ -622,10 +616,10 @@
     <t>User could still run with no input. Conditional statement placed that checks if the input value is not null</t>
   </si>
   <si>
-    <t>ME</t>
-  </si>
-  <si>
-    <t>Local: CD</t>
+    <t>User could use number selector and pick number over 99. Max set to 99</t>
+  </si>
+  <si>
+    <t>Code</t>
   </si>
 </sst>
 </file>
@@ -928,6 +922,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -943,7 +938,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1285,7 +1279,7 @@
   <dimension ref="A1:H57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1353,17 +1347,17 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="23">
+      <c r="A7" s="18">
         <v>43549</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7" t="s">
-        <v>67</v>
+      <c r="C7">
+        <v>70</v>
       </c>
       <c r="D7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -1372,21 +1366,21 @@
         <v>1</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="23">
+      <c r="A8" s="18">
         <v>43549</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
-      <c r="C8" t="s">
-        <v>69</v>
+      <c r="C8">
+        <v>60</v>
       </c>
       <c r="D8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -1395,21 +1389,21 @@
         <v>2</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="23">
+      <c r="A9" s="18">
         <v>43549</v>
       </c>
       <c r="B9">
         <v>3</v>
       </c>
-      <c r="C9" t="s">
-        <v>69</v>
+      <c r="C9">
+        <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -1418,21 +1412,21 @@
         <v>3</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="23">
+      <c r="A10" s="18">
         <v>43549</v>
       </c>
       <c r="B10">
         <v>4</v>
       </c>
-      <c r="C10" t="s">
-        <v>73</v>
+      <c r="C10">
+        <v>60</v>
       </c>
       <c r="D10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -1441,23 +1435,31 @@
         <v>4</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="23">
+      <c r="A11" s="18">
         <v>43549</v>
       </c>
       <c r="B11">
         <v>5</v>
       </c>
+      <c r="C11">
+        <v>60</v>
+      </c>
+      <c r="D11" t="s">
+        <v>72</v>
+      </c>
       <c r="F11">
         <v>1</v>
       </c>
       <c r="G11">
         <v>5</v>
       </c>
-      <c r="H11" s="6"/>
+      <c r="H11" s="6" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H12" s="6"/>
@@ -1623,7 +1625,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="19" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -1631,13 +1633,13 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="19"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="9" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="19" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -1645,13 +1647,13 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="20"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="9" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -1659,19 +1661,19 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="19"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="11" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="19" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="9" t="s">
@@ -1679,7 +1681,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="19"/>
+      <c r="A10" s="20"/>
       <c r="B10" s="11" t="s">
         <v>25</v>
       </c>
@@ -1693,7 +1695,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B12" s="9" t="s">
@@ -1701,13 +1703,13 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="19"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="11" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="19" t="s">
         <v>5</v>
       </c>
       <c r="B14" s="9" t="s">
@@ -1715,13 +1717,13 @@
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="19"/>
+      <c r="A15" s="20"/>
       <c r="B15" s="11" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="19" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="9" t="s">
@@ -1729,7 +1731,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="19"/>
+      <c r="A17" s="20"/>
       <c r="B17" s="11" t="s">
         <v>33</v>
       </c>
@@ -1743,7 +1745,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="19" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="9" t="s">
@@ -1751,13 +1753,13 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="19"/>
+      <c r="A20" s="20"/>
       <c r="B20" s="11" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="19" t="s">
         <v>37</v>
       </c>
       <c r="B21" s="9" t="s">
@@ -1765,7 +1767,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="19"/>
+      <c r="A22" s="20"/>
       <c r="B22" s="11" t="s">
         <v>39</v>
       </c>

</xml_diff>